<commit_message>
refactor, docs: changes folder structures and code structures, makes README.md with full explaination
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>q3</t>
+          <t>q1</t>
         </is>
       </c>
     </row>
@@ -478,12 +478,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>∅</t>
+          <t>q2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>q1</t>
+          <t>q3</t>
         </is>
       </c>
     </row>
@@ -495,72 +495,89 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>∅</t>
+          <t>q2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>∅</t>
+          <t>q4</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>q4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>q1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Q :</t>
+          <t> </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{q1,q2,q3}</t>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Σ : </t>
+          <t>Q :</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{a,b}</t>
+          <t>{q1,q2,q3,q4}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Start : </t>
+          <t xml:space="preserve">Σ : </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>q1</t>
+          <t>{a,b}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t xml:space="preserve">Start : </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t xml:space="preserve">Accept : </t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>{q2,q3}</t>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>{q4}</t>
         </is>
       </c>
     </row>

</xml_diff>